<commit_message>
Update monthly cost analysis and export estimate file
</commit_message>
<xml_diff>
--- a/ExportedEstimate.xlsx
+++ b/ExportedEstimate.xlsx
@@ -53,7 +53,7 @@
     <t>Southeast Asia</t>
   </si>
   <si>
-    <t>Single Server Deployment, Basic Tier, 1 Gen 5 (1 vCore) x 730 Hours, 5 GiB Storage, 1 GiB Additional Backup storage - LRS redundancy</t>
+    <t>Single Server Deployment, General Purpose Tier, 1 Gen 5 (2 vCore) x 730 Hours, 20 GiB Storage, 50 GiB Additional Backup storage - LRS redundancy</t>
   </si>
   <si>
     <t>Integration</t>
@@ -62,7 +62,7 @@
     <t>Service Bus</t>
   </si>
   <si>
-    <t>Basic tier: 1 million messaging operations</t>
+    <t>Standard tier: Messaging Operations: 730 Hours of base charge, 1 x 1 million operations; 0 brokered connection(s); Hybrid Connections: 0 listener(s), 0 overage GB; WFC Relays: 0 x 100 relay hours, 0 x 10,000 message(s)</t>
   </si>
   <si>
     <t>Compute</t>
@@ -71,7 +71,7 @@
     <t>App Service</t>
   </si>
   <si>
-    <t>Basic Tier; 1 B1 (1 Core(s), 1.75 GB RAM, 10 GB Storage) x 730 Hours; Linux OS; 0 SNI SSL Connections; 0 IP SSL Connections</t>
+    <t>Standard Tier; 1 S2 (2 Core(s), 3.5 GB RAM, 50 GB Storage) x 730 Hours; Linux OS; 0 SNI SSL Connections; 0 IP SSL Connections</t>
   </si>
   <si>
     <t>Storage</t>
@@ -86,7 +86,7 @@
     <t>Azure Functions</t>
   </si>
   <si>
-    <t>Consumption tier, Pay as you go, 128 MB memory, 100 milliseconds execution time, 1,000,000 executions/mo</t>
+    <t>Consumption tier, Pay as you go, 128 MB memory, 100 milliseconds execution time, 0 executions/mo</t>
   </si>
   <si>
     <t>Support</t>
@@ -113,7 +113,7 @@
     <t>All prices shown are in United States – Dollar ($) USD. This is a summary estimate, not a quote. For up to date pricing information please visit https://azure.microsoft.com/pricing/calculator/</t>
   </si>
   <si>
-    <t>This estimate was created at 4/14/2023 8:35:52 PM UTC.</t>
+    <t>This estimate was created at 4/15/2023 1:41:33 AM UTC.</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="5">
-        <v>39.71</v>
+        <v>84.12</v>
       </c>
       <c r="G4" s="5">
         <v>0</v>
@@ -428,7 +428,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="5">
-        <v>0.05</v>
+        <v>9.81193</v>
       </c>
       <c r="G5" s="5">
         <v>0</v>
@@ -470,7 +470,7 @@
         <v>19</v>
       </c>
       <c r="F6" s="5">
-        <v>13.14</v>
+        <v>138.7</v>
       </c>
       <c r="G6" s="5">
         <v>0</v>
@@ -720,7 +720,7 @@
       </c>
       <c r="E13" s="14"/>
       <c r="F13" s="15">
-        <v>55.944</v>
+        <v>235.67593</v>
       </c>
       <c r="G13" s="15">
         <v>0</v>

</xml_diff>